<commit_message>
updated ch1 quiz and ch2 hw
</commit_message>
<xml_diff>
--- a/algebraI/gradebook.xlsx
+++ b/algebraI/gradebook.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Projects/math_tutoring/algebraI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910F0857-BDCB-8C42-87D7-C76866786A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3E9863-73BB-EB4E-9F22-6551B1B1EC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{47081AD2-0D95-E54A-9257-08E2F0321F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="AlgebraI" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Homework</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Chapter 1 Grade</t>
+  </si>
+  <si>
+    <t>Assignments and Grades Received - Chapter 2</t>
   </si>
 </sst>
 </file>
@@ -570,91 +573,91 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -971,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D10EC-0B06-534D-B943-04716498664F}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,39 +988,39 @@
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23" t="s">
+      <c r="I3" s="35"/>
+      <c r="J3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1026,22 +1029,22 @@
       <c r="C4" s="4">
         <v>5</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1052,20 +1055,24 @@
       <c r="C5" s="6">
         <v>40</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="21">
         <v>100</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31" t="s">
+      <c r="I5" s="21">
+        <v>100</v>
+      </c>
+      <c r="J5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="32"/>
+      <c r="K5" s="22">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
@@ -1074,13 +1081,13 @@
       <c r="C6" s="8">
         <v>25</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1099,52 +1106,169 @@
         <f>SUM(C4:C7)</f>
         <v>100</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="35" t="s">
+      <c r="G8" s="39"/>
+      <c r="H8" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="35" t="s">
+      <c r="I8" s="39"/>
+      <c r="J8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="36"/>
+      <c r="K8" s="39"/>
     </row>
     <row r="9" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="37">
+      <c r="F9" s="25">
         <f>AVERAGE(G5:G6)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="37" t="e">
+      <c r="G9" s="26"/>
+      <c r="H9" s="25">
         <f>AVERAGE(I5:I6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="37" t="e">
-        <f t="shared" ref="J9:K9" si="0">AVERAGE(K5:K6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="38"/>
+        <v>100</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="25">
+        <f t="shared" ref="J9" si="0">AVERAGE(K5:K6)</f>
+        <v>101</v>
+      </c>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="39" t="e">
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="27">
         <f>F9*0.4+H9*0.25+J9*0.3+5</f>
+        <v>100.3</v>
+      </c>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F14" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="37"/>
+    </row>
+    <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="21">
+        <v>94</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="22"/>
+    </row>
+    <row r="17" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F19" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="39"/>
+    </row>
+    <row r="20" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="25">
+        <f>AVERAGE(G16:G17)</f>
+        <v>94</v>
+      </c>
+      <c r="G20" s="26"/>
+      <c r="H20" s="25" t="e">
+        <f>AVERAGE(I16:I17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="41"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="25" t="e">
+        <f t="shared" ref="J20" si="1">AVERAGE(K16:K17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="6:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="27" t="e">
+        <f>F20*0.4+H20*0.25+J20*0.3+5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="25">
     <mergeCell ref="F11:I11"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="F8:G8"/>
@@ -1158,6 +1282,18 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added first hw grade
</commit_message>
<xml_diff>
--- a/algebraI/gradebook.xlsx
+++ b/algebraI/gradebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Projects/math_tutoring/algebraI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FB16A9-FAA3-ED47-AA6E-62C7EB628FA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C2428-53A2-4740-A8F8-36164C749BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{47081AD2-0D95-E54A-9257-08E2F0321F5A}"/>
   </bookViews>
@@ -663,6 +663,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,21 +693,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,15 +721,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D10EC-0B06-534D-B943-04716498664F}">
   <dimension ref="B1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,19 +1051,19 @@
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="41"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
@@ -1072,18 +1072,18 @@
       <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="39"/>
+      <c r="K3" s="42"/>
     </row>
     <row r="4" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1169,74 +1169,74 @@
         <f>SUM(C4:C7)</f>
         <v>100</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="32"/>
+      <c r="H8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="29"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="30">
+      <c r="F9" s="33">
         <f>AVERAGE(G5:G6)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="30">
+      <c r="G9" s="34"/>
+      <c r="H9" s="33">
         <f>AVERAGE(I5:I6)</f>
         <v>100</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="30">
+      <c r="I9" s="34"/>
+      <c r="J9" s="33">
         <f t="shared" ref="J9" si="0">AVERAGE(K5:K6)</f>
         <v>101</v>
       </c>
-      <c r="K9" s="31"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="25">
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="28">
         <f>F9*0.4+H9*0.25+J9*0.3+5</f>
         <v>100.3</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="37" t="s">
+      <c r="G14" s="39"/>
+      <c r="H14" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38" t="s">
+      <c r="I14" s="40"/>
+      <c r="J14" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="39"/>
+      <c r="K14" s="42"/>
     </row>
     <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="15" t="s">
@@ -1292,74 +1292,74 @@
     </row>
     <row r="18" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="28" t="s">
+      <c r="G19" s="32"/>
+      <c r="H19" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="28" t="s">
+      <c r="I19" s="32"/>
+      <c r="J19" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="29"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="30">
+      <c r="F20" s="33">
         <f>AVERAGE(G16:G17)</f>
         <v>95.25</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="30">
+      <c r="G20" s="34"/>
+      <c r="H20" s="33">
         <f>AVERAGE(I16:I17)</f>
         <v>94</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="30">
+      <c r="I20" s="34"/>
+      <c r="J20" s="33">
         <f t="shared" ref="J20" si="1">AVERAGE(K16:K17)</f>
         <v>93</v>
       </c>
-      <c r="K20" s="31"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="6:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="25">
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="28">
         <f>F20*0.4+H20*0.25+J20*0.3+5</f>
         <v>94.5</v>
       </c>
-      <c r="K22" s="27"/>
+      <c r="K22" s="30"/>
     </row>
     <row r="23" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="6:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="37" t="s">
+      <c r="G25" s="39"/>
+      <c r="H25" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="38" t="s">
+      <c r="I25" s="40"/>
+      <c r="J25" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K25" s="39"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F26" s="15" t="s">
@@ -1415,49 +1415,49 @@
     </row>
     <row r="29" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="28" t="s">
+      <c r="G30" s="32"/>
+      <c r="H30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="28" t="s">
+      <c r="I30" s="32"/>
+      <c r="J30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="29"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="30">
+      <c r="F31" s="33">
         <f>AVERAGE(G27:G28)</f>
         <v>99</v>
       </c>
-      <c r="G31" s="31"/>
-      <c r="H31" s="30">
+      <c r="G31" s="34"/>
+      <c r="H31" s="33">
         <f>AVERAGE(I27:I28)</f>
         <v>91</v>
       </c>
-      <c r="I31" s="31"/>
-      <c r="J31" s="30">
+      <c r="I31" s="34"/>
+      <c r="J31" s="33">
         <f t="shared" ref="J31" si="2">AVERAGE(K27:K28)</f>
         <v>91</v>
       </c>
-      <c r="K31" s="31"/>
+      <c r="K31" s="34"/>
     </row>
     <row r="32" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="6:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="25" t="s">
+      <c r="F33" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="25">
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="28">
         <f>F31*0.4+H31*0.25+J31*0.3+5</f>
         <v>94.65</v>
       </c>
-      <c r="K33" s="27"/>
+      <c r="K33" s="30"/>
     </row>
     <row r="34" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="O34" t="s">
@@ -1465,28 +1465,28 @@
       </c>
     </row>
     <row r="35" spans="6:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
     </row>
     <row r="36" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="37" t="s">
+      <c r="G36" s="39"/>
+      <c r="H36" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="38" t="s">
+      <c r="I36" s="40"/>
+      <c r="J36" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="39"/>
+      <c r="K36" s="42"/>
     </row>
     <row r="37" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F37" s="15" t="s">
@@ -1512,7 +1512,10 @@
       <c r="F38" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="21"/>
+      <c r="G38" s="21">
+        <f>AVERAGE(100,99,98)</f>
+        <v>99</v>
+      </c>
       <c r="H38" s="21" t="s">
         <v>19</v>
       </c>
@@ -1525,14 +1528,14 @@
       <c r="K38" s="22"/>
     </row>
     <row r="39" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="44"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="27"/>
     </row>
     <row r="40" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F40" s="23" t="s">
@@ -1546,60 +1549,84 @@
     </row>
     <row r="41" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="29"/>
-      <c r="H42" s="28" t="s">
+      <c r="G42" s="32"/>
+      <c r="H42" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="29"/>
-      <c r="J42" s="28" t="s">
+      <c r="I42" s="32"/>
+      <c r="J42" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K42" s="29"/>
+      <c r="K42" s="32"/>
     </row>
     <row r="43" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F43" s="30" t="e">
+      <c r="F43" s="33">
         <f>AVERAGE(G38:G40)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G43" s="31"/>
-      <c r="H43" s="30">
+        <v>99</v>
+      </c>
+      <c r="G43" s="34"/>
+      <c r="H43" s="33">
         <f>AVERAGE(I38:I40)</f>
         <v>98</v>
       </c>
-      <c r="I43" s="31"/>
-      <c r="J43" s="30" t="e">
-        <f t="shared" ref="J43" si="3">AVERAGE(K38:K40)</f>
+      <c r="I43" s="34"/>
+      <c r="J43" s="33" t="e">
+        <f>AVERAGE(K38:K40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K43" s="31"/>
+      <c r="K43" s="34"/>
     </row>
     <row r="44" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="6:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="25" t="s">
+      <c r="F45" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="25" t="e">
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="28" t="e">
         <f>F43*0.4+H43*0.25+J43*0.3+5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K45" s="27"/>
+      <c r="K45" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="F35:K35"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="H36:I36"/>
@@ -1609,38 +1636,14 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="J33:K33"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:K43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Final chapter 5 grades
</commit_message>
<xml_diff>
--- a/algebraI/gradebook.xlsx
+++ b/algebraI/gradebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Projects/math_tutoring/algebraI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2C1DE-5A22-E842-9A8E-38CC6C68FA73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D17188-84C8-6F48-8290-51193E144E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{47081AD2-0D95-E54A-9257-08E2F0321F5A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
   <si>
     <t>Homework</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Assignments and Grades Received - Chapter 5</t>
+  </si>
+  <si>
+    <t>Assignments and Grades Received - Chapter 6</t>
+  </si>
+  <si>
+    <t>Chapter 6 Grade</t>
   </si>
 </sst>
 </file>
@@ -681,6 +687,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -690,40 +702,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1046,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D10EC-0B06-534D-B943-04716498664F}">
-  <dimension ref="B1:O58"/>
+  <dimension ref="B1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,14 +1071,14 @@
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
@@ -1081,18 +1087,18 @@
       <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="40" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="42"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1178,74 +1184,74 @@
         <f>SUM(C4:C7)</f>
         <v>100</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="31" t="s">
+      <c r="G8" s="42"/>
+      <c r="H8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="31" t="s">
+      <c r="I8" s="42"/>
+      <c r="J8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="42"/>
     </row>
     <row r="9" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="33">
+      <c r="F9" s="28">
         <f>AVERAGE(G5:G6)</f>
         <v>100</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="33">
+      <c r="G9" s="29"/>
+      <c r="H9" s="28">
         <f>AVERAGE(I5:I6)</f>
         <v>100</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="33">
+      <c r="I9" s="29"/>
+      <c r="J9" s="28">
         <f t="shared" ref="J9" si="0">AVERAGE(K5:K6)</f>
         <v>101</v>
       </c>
-      <c r="K9" s="34"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="28">
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30">
         <f>F9*0.4+H9*0.25+J9*0.3+5</f>
         <v>100.3</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="39"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="40" t="s">
+      <c r="G14" s="37"/>
+      <c r="H14" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41" t="s">
+      <c r="I14" s="38"/>
+      <c r="J14" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="42"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F15" s="15" t="s">
@@ -1301,74 +1307,74 @@
     </row>
     <row r="18" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="31" t="s">
+      <c r="G19" s="42"/>
+      <c r="H19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="32"/>
-      <c r="J19" s="31" t="s">
+      <c r="I19" s="42"/>
+      <c r="J19" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="42"/>
     </row>
     <row r="20" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="33">
+      <c r="F20" s="28">
         <f>AVERAGE(G16:G17)</f>
         <v>95.25</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33">
+      <c r="G20" s="29"/>
+      <c r="H20" s="28">
         <f>AVERAGE(I16:I17)</f>
         <v>94</v>
       </c>
-      <c r="I20" s="34"/>
-      <c r="J20" s="33">
+      <c r="I20" s="29"/>
+      <c r="J20" s="28">
         <f t="shared" ref="J20" si="1">AVERAGE(K16:K17)</f>
         <v>93</v>
       </c>
-      <c r="K20" s="34"/>
+      <c r="K20" s="29"/>
     </row>
     <row r="21" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="6:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="28">
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="30">
         <f>F20*0.4+H20*0.25+J20*0.3+5</f>
         <v>94.5</v>
       </c>
-      <c r="K22" s="30"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="6:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="35"/>
     </row>
     <row r="25" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="40" t="s">
+      <c r="G25" s="37"/>
+      <c r="H25" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41" t="s">
+      <c r="I25" s="38"/>
+      <c r="J25" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K25" s="42"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F26" s="15" t="s">
@@ -1424,49 +1430,49 @@
     </row>
     <row r="29" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="31" t="s">
+      <c r="G30" s="42"/>
+      <c r="H30" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="32"/>
-      <c r="J30" s="31" t="s">
+      <c r="I30" s="42"/>
+      <c r="J30" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="32"/>
+      <c r="K30" s="42"/>
     </row>
     <row r="31" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="33">
+      <c r="F31" s="28">
         <f>AVERAGE(G27:G28)</f>
         <v>99</v>
       </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="33">
+      <c r="G31" s="29"/>
+      <c r="H31" s="28">
         <f>AVERAGE(I27:I28)</f>
         <v>91</v>
       </c>
-      <c r="I31" s="34"/>
-      <c r="J31" s="33">
+      <c r="I31" s="29"/>
+      <c r="J31" s="28">
         <f t="shared" ref="J31" si="2">AVERAGE(K27:K28)</f>
         <v>91</v>
       </c>
-      <c r="K31" s="34"/>
+      <c r="K31" s="29"/>
     </row>
     <row r="32" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="6:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="28">
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="30">
         <f>F31*0.4+H31*0.25+J31*0.3+5</f>
         <v>94.65</v>
       </c>
-      <c r="K33" s="30"/>
+      <c r="K33" s="32"/>
     </row>
     <row r="34" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="O34" t="s">
@@ -1474,28 +1480,28 @@
       </c>
     </row>
     <row r="35" spans="6:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="37" t="s">
+      <c r="F35" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="39"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="35"/>
     </row>
     <row r="36" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="40" t="s">
+      <c r="G36" s="37"/>
+      <c r="H36" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="41" t="s">
+      <c r="I36" s="38"/>
+      <c r="J36" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="42"/>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F37" s="15" t="s">
@@ -1558,74 +1564,74 @@
     </row>
     <row r="41" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="32"/>
-      <c r="H42" s="31" t="s">
+      <c r="G42" s="42"/>
+      <c r="H42" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="31" t="s">
+      <c r="I42" s="42"/>
+      <c r="J42" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K42" s="32"/>
+      <c r="K42" s="42"/>
     </row>
     <row r="43" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F43" s="33">
+      <c r="F43" s="28">
         <f>AVERAGE(G38:G40)</f>
         <v>99</v>
       </c>
-      <c r="G43" s="34"/>
-      <c r="H43" s="33">
+      <c r="G43" s="29"/>
+      <c r="H43" s="28">
         <f>AVERAGE(I38:I40)</f>
         <v>98</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="33" t="e">
+      <c r="I43" s="29"/>
+      <c r="J43" s="28" t="e">
         <f>AVERAGE(K38:K40)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K43" s="34"/>
+      <c r="K43" s="29"/>
     </row>
     <row r="44" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="6:15" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="28" t="s">
+      <c r="F45" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="28" t="e">
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="30" t="e">
         <f>F43*0.4+H43*0.25+J43*0.3+5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K45" s="30"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="6:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="6:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="39"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="35"/>
     </row>
     <row r="48" spans="6:15" x14ac:dyDescent="0.2">
-      <c r="F48" s="35" t="s">
+      <c r="F48" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="40" t="s">
+      <c r="G48" s="37"/>
+      <c r="H48" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="41" t="s">
+      <c r="I48" s="38"/>
+      <c r="J48" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K48" s="42"/>
+      <c r="K48" s="40"/>
     </row>
     <row r="49" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F49" s="15" t="s">
@@ -1664,7 +1670,7 @@
         <v>20</v>
       </c>
       <c r="K50" s="22">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="6:11" x14ac:dyDescent="0.2">
@@ -1703,72 +1709,241 @@
     </row>
     <row r="54" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G55" s="32"/>
-      <c r="H55" s="31" t="s">
+      <c r="G55" s="42"/>
+      <c r="H55" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I55" s="32"/>
-      <c r="J55" s="31" t="s">
+      <c r="I55" s="42"/>
+      <c r="J55" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K55" s="32"/>
+      <c r="K55" s="42"/>
     </row>
     <row r="56" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F56" s="33">
+      <c r="F56" s="28">
         <f>AVERAGE(G50:G53)</f>
         <v>98</v>
       </c>
-      <c r="G56" s="34"/>
-      <c r="H56" s="33">
+      <c r="G56" s="29"/>
+      <c r="H56" s="28">
         <f>AVERAGE(I50:I53)</f>
         <v>100</v>
       </c>
-      <c r="I56" s="34"/>
-      <c r="J56" s="33">
+      <c r="I56" s="29"/>
+      <c r="J56" s="28">
         <f>AVERAGE(K50:K53)</f>
-        <v>0</v>
-      </c>
-      <c r="K56" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="K56" s="29"/>
     </row>
     <row r="57" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="6:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="28" t="s">
+      <c r="F58" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="28">
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="30">
         <f>F56*0.4+H56*0.25+J56*0.3+5</f>
-        <v>69.2</v>
-      </c>
-      <c r="K58" s="30"/>
+        <v>98</v>
+      </c>
+      <c r="K58" s="32"/>
+    </row>
+    <row r="59" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="6:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="35"/>
+    </row>
+    <row r="61" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F61" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="G61" s="37"/>
+      <c r="H61" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" s="38"/>
+      <c r="J61" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="K61" s="40"/>
+    </row>
+    <row r="62" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I62" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J62" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F63" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="21">
+        <v>97</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" s="21">
+        <v>100</v>
+      </c>
+      <c r="J63" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" s="22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F64" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="26">
+        <v>98</v>
+      </c>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="27"/>
+    </row>
+    <row r="65" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F65" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="26">
+        <v>99</v>
+      </c>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="27"/>
+    </row>
+    <row r="66" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="2"/>
+    </row>
+    <row r="67" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F68" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="42"/>
+      <c r="H68" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" s="42"/>
+      <c r="J68" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K68" s="42"/>
+    </row>
+    <row r="69" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F69" s="28">
+        <f>AVERAGE(G63:G66)</f>
+        <v>98</v>
+      </c>
+      <c r="G69" s="29"/>
+      <c r="H69" s="28">
+        <f>AVERAGE(I63:I66)</f>
+        <v>100</v>
+      </c>
+      <c r="I69" s="29"/>
+      <c r="J69" s="28">
+        <f>AVERAGE(K63:K66)</f>
+        <v>96</v>
+      </c>
+      <c r="K69" s="29"/>
+    </row>
+    <row r="70" spans="6:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="6:11" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F71" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="30">
+        <f>F69*0.4+H69*0.25+J69*0.3+5</f>
+        <v>98</v>
+      </c>
+      <c r="K71" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="F47:K47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
+  <mergeCells count="73">
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="F60:K60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="F35:K35"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="H36:I36"/>
@@ -1778,38 +1953,26 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="J33:K33"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="F47:K47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="J58:K58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>